<commit_message>
Upload RC & RLC data
</commit_message>
<xml_diff>
--- a/LO6/FP/data.xlsx
+++ b/LO6/FP/data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinplanck/Desktop/Physics/Physics Lab III/LO6/FP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC35C67D-36A6-EB4D-9BC7-0F50FFECDE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94F4668-107C-F64C-844B-5AF60FF7D9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{B143CE9D-3D72-9F41-B454-706F6D1BF283}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>dlambda (rel.)</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>d2</t>
-  </si>
-  <si>
-    <t>estimeshon</t>
   </si>
 </sst>
 </file>
@@ -66,12 +63,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,8 +101,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225C3F64-BAE6-0A4A-9859-C0C594C3D72F}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="B1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -413,18 +431,18 @@
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C1">
         <f>10/5</f>
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>0.58930000000000005</v>
       </c>
@@ -436,7 +454,7 @@
         <v>67.877142372306125</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -447,7 +465,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -458,63 +476,204 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B8" s="2">
         <f>40/69</f>
         <v>0.57971014492753625</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <f>2*20/68</f>
         <v>0.58823529411764708</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9">
+      <c r="D8" s="2">
+        <f>C8 * 0.1003</f>
+        <v>5.9000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
         <v>1000</v>
+      </c>
+      <c r="C9" s="1">
+        <f>C8*1000</f>
+        <v>588.23529411764707</v>
+      </c>
+      <c r="D9" s="1">
+        <f>D8*1000</f>
+        <v>59.000000000000007</v>
       </c>
       <c r="F9">
         <v>845</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10">
+      <c r="I9">
+        <v>1110</v>
+      </c>
+      <c r="L9">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
         <v>845</v>
       </c>
-      <c r="D10">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
         <f>B3^2/(2*B11)</f>
         <v>5.6012014516129043E-3</v>
       </c>
       <c r="F10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <f>(B9-B10)/5</f>
+      <c r="I10">
+        <v>922</v>
+      </c>
+      <c r="J10">
+        <f>(I10 - I9)/5</f>
+        <v>-37.6</v>
+      </c>
+      <c r="K10">
+        <f>J10*10</f>
+        <v>-376</v>
+      </c>
+      <c r="L10">
+        <v>1306</v>
+      </c>
+      <c r="M10">
+        <f>(L10-L9)/5</f>
+        <v>39.200000000000003</v>
+      </c>
+      <c r="N10">
+        <f>M10*10</f>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <f>ABS(B9-B10)/5</f>
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13">
+      <c r="C11" s="1">
+        <f>B11*10</f>
+        <v>310</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="J13" s="1">
+        <f>$C$8^2/(J10*2)</f>
+        <v>-4.6013399101818451E-3</v>
+      </c>
+      <c r="N13" s="1">
+        <f>$C$8^2/(N10*2)</f>
+        <v>4.4135301179295253E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="3">
         <v>1168</v>
       </c>
-      <c r="D14">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
         <f>B3^2/(2*B15)</f>
         <v>5.1677751488095241E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15">
+      <c r="E14" s="1">
+        <f>$C$8^2/(C11*2)</f>
+        <v>5.5809800200915286E-4</v>
+      </c>
+      <c r="F14" s="1">
+        <f>$C$8/(2*C11) * SQRT(4*$D$8^2 +( $C$8/C11 * $D$25)^2)</f>
+        <v>1.1195445972414516E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="3">
         <f>ABS(B13-B14)/5</f>
         <v>33.6</v>
+      </c>
+      <c r="C15" s="3">
+        <f>B15*10</f>
+        <v>336</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1">
+        <f>E14*1000</f>
+        <v>0.55809800200915283</v>
+      </c>
+      <c r="F15" s="1">
+        <f>F14*1000</f>
+        <v>0.11195445972414517</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <f>AVERAGE(E15,E20)</f>
+        <v>0.53650492455046539</v>
+      </c>
+      <c r="H17">
+        <f>_xlfn.T.INV.2T(0.05, 1)*_xlfn.STDEV.S(E15,E20)/SQRT(2)</f>
+        <v>0.27436606307416161</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f>1000-845</f>
+        <v>155</v>
+      </c>
+      <c r="D19">
+        <f>SQRT(0.02^2 + 0.02^2)</f>
+        <v>2.8284271247461901E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <f>$C$8^2/(C15*2)</f>
+        <v>5.1491184709177797E-4</v>
+      </c>
+      <c r="F19" s="3">
+        <f>$C$8/(2*C15) * SQRT(4*$D$8^2 +( $C$8/C15 * $D$25)^2)</f>
+        <v>1.0329131693586745E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f>B14-B13</f>
+        <v>168</v>
+      </c>
+      <c r="E20" s="3">
+        <f>E19*1000</f>
+        <v>0.51491184709177795</v>
+      </c>
+      <c r="F20" s="3">
+        <f>F19*1000</f>
+        <v>0.10329131693586746</v>
+      </c>
+      <c r="G20">
+        <f>(E15/F15^2 + E20/F20^2)/SUM(1/F15^2+1/F20^2)</f>
+        <v>0.53476959309866223</v>
+      </c>
+      <c r="H20">
+        <f>SQRT(1/SUM(1/F15^2+1/F20^2))</f>
+        <v>7.59161377290338E-2</v>
+      </c>
+      <c r="I20">
+        <f>(H20^2+H17^2)^0.5</f>
+        <v>0.28467524749178397</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <f>I20/G20</f>
+        <v>0.53233252444714607</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f>0.03 / 5</f>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>